<commit_message>
Atualizacao diaria Wizard Lotofacil (jogos + backtest + dashboard + relatorios)
</commit_message>
<xml_diff>
--- a/base/base_dados_atualizada.xlsx
+++ b/base/base_dados_atualizada.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -434,87 +422,87 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Concurso</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>D1</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>D2</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>D3</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>D4</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>D5</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>D6</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>D7</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>D8</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>D9</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>D10</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>D11</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>D12</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>D13</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>D14</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>D15</t>
         </is>

</xml_diff>

<commit_message>
Atualizacao diaria Wizard Lotofacil
</commit_message>
<xml_diff>
--- a/base/base_dados_atualizada.xlsx
+++ b/base/base_dados_atualizada.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q1000"/>
+  <dimension ref="A1:Q1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -53970,42 +53970,42 @@
     </row>
     <row r="974">
       <c r="A974" t="n">
-        <v>3589</v>
+        <v>3588</v>
       </c>
       <c r="B974" t="inlineStr">
         <is>
-          <t>16/01/2026</t>
+          <t>15/01/2026</t>
         </is>
       </c>
       <c r="C974" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D974" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E974" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F974" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G974" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H974" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I974" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="J974" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K974" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L974" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M974" t="n">
         <v>19</v>
@@ -54017,194 +54017,194 @@
         <v>22</v>
       </c>
       <c r="P974" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q974" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="975">
       <c r="A975" t="n">
-        <v>3590</v>
+        <v>3589</v>
       </c>
       <c r="B975" t="inlineStr">
         <is>
-          <t>17/01/2026</t>
+          <t>16/01/2026</t>
         </is>
       </c>
       <c r="C975" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D975" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E975" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F975" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G975" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H975" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I975" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J975" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K975" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L975" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M975" t="n">
         <v>19</v>
       </c>
       <c r="N975" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O975" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P975" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="Q975" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="976">
       <c r="A976" t="n">
-        <v>3591</v>
+        <v>3590</v>
       </c>
       <c r="B976" t="inlineStr">
         <is>
-          <t>19/01/2026</t>
+          <t>17/01/2026</t>
         </is>
       </c>
       <c r="C976" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D976" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E976" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F976" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G976" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H976" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="I976" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J976" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="K976" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L976" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="M976" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="N976" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="O976" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="P976" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="Q976" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="977">
       <c r="A977" t="n">
-        <v>3592</v>
+        <v>3591</v>
       </c>
       <c r="B977" t="inlineStr">
         <is>
-          <t>20/01/2026</t>
+          <t>19/01/2026</t>
         </is>
       </c>
       <c r="C977" t="n">
         <v>1</v>
       </c>
       <c r="D977" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E977" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F977" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G977" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H977" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I977" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J977" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K977" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="L977" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="M977" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="N977" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="O977" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="P977" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="Q977" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="978">
       <c r="A978" t="n">
-        <v>3593</v>
+        <v>3592</v>
       </c>
       <c r="B978" t="inlineStr">
         <is>
-          <t>21/01/2026</t>
+          <t>20/01/2026</t>
         </is>
       </c>
       <c r="C978" t="n">
         <v>1</v>
       </c>
       <c r="D978" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E978" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F978" t="n">
         <v>6</v>
@@ -54213,31 +54213,31 @@
         <v>7</v>
       </c>
       <c r="H978" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I978" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J978" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="K978" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="L978" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="M978" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="N978" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="O978" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P978" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q978" t="n">
         <v>25</v>
@@ -54245,24 +54245,24 @@
     </row>
     <row r="979">
       <c r="A979" t="n">
-        <v>3594</v>
+        <v>3593</v>
       </c>
       <c r="B979" t="inlineStr">
         <is>
-          <t>22/01/2026</t>
+          <t>21/01/2026</t>
         </is>
       </c>
       <c r="C979" t="n">
         <v>1</v>
       </c>
       <c r="D979" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E979" t="n">
         <v>4</v>
       </c>
       <c r="F979" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G979" t="n">
         <v>7</v>
@@ -54274,10 +54274,10 @@
         <v>9</v>
       </c>
       <c r="J979" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K979" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L979" t="n">
         <v>15</v>
@@ -54286,25 +54286,25 @@
         <v>18</v>
       </c>
       <c r="N979" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O979" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="P979" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q979" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="980">
       <c r="A980" t="n">
-        <v>3595</v>
+        <v>3594</v>
       </c>
       <c r="B980" t="inlineStr">
         <is>
-          <t>23/01/2026</t>
+          <t>22/01/2026</t>
         </is>
       </c>
       <c r="C980" t="n">
@@ -54320,25 +54320,25 @@
         <v>5</v>
       </c>
       <c r="G980" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H980" t="n">
         <v>8</v>
       </c>
       <c r="I980" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J980" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K980" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L980" t="n">
         <v>15</v>
       </c>
       <c r="M980" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="N980" t="n">
         <v>20</v>
@@ -54347,19 +54347,19 @@
         <v>21</v>
       </c>
       <c r="P980" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Q980" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="981">
       <c r="A981" t="n">
-        <v>3596</v>
+        <v>3595</v>
       </c>
       <c r="B981" t="inlineStr">
         <is>
-          <t>24/01/2026</t>
+          <t>23/01/2026</t>
         </is>
       </c>
       <c r="C981" t="n">
@@ -54369,25 +54369,25 @@
         <v>2</v>
       </c>
       <c r="E981" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F981" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G981" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H981" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I981" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J981" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="K981" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L981" t="n">
         <v>15</v>
@@ -54396,175 +54396,175 @@
         <v>16</v>
       </c>
       <c r="N981" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="O981" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P981" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q981" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="982">
       <c r="A982" t="n">
-        <v>3597</v>
+        <v>3596</v>
       </c>
       <c r="B982" t="inlineStr">
         <is>
-          <t>26/01/2026</t>
+          <t>24/01/2026</t>
         </is>
       </c>
       <c r="C982" t="n">
         <v>1</v>
       </c>
       <c r="D982" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E982" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F982" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G982" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H982" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="I982" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J982" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="K982" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L982" t="n">
+        <v>15</v>
+      </c>
+      <c r="M982" t="n">
         <v>16</v>
       </c>
-      <c r="M982" t="n">
-        <v>19</v>
-      </c>
       <c r="N982" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="O982" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P982" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Q982" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="983">
       <c r="A983" t="n">
-        <v>3598</v>
+        <v>3597</v>
       </c>
       <c r="B983" t="inlineStr">
         <is>
-          <t>27/01/2026</t>
+          <t>26/01/2026</t>
         </is>
       </c>
       <c r="C983" t="n">
         <v>1</v>
       </c>
       <c r="D983" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E983" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F983" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G983" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H983" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I983" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="J983" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="K983" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="L983" t="n">
         <v>16</v>
       </c>
       <c r="M983" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N983" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O983" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P983" t="n">
         <v>23</v>
       </c>
       <c r="Q983" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="984">
       <c r="A984" t="n">
-        <v>3599</v>
+        <v>3598</v>
       </c>
       <c r="B984" t="inlineStr">
         <is>
-          <t>28/01/2026</t>
+          <t>27/01/2026</t>
         </is>
       </c>
       <c r="C984" t="n">
         <v>1</v>
       </c>
       <c r="D984" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E984" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F984" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G984" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H984" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I984" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J984" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="K984" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="L984" t="n">
         <v>16</v>
       </c>
       <c r="M984" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N984" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O984" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P984" t="n">
         <v>23</v>
@@ -54575,45 +54575,45 @@
     </row>
     <row r="985">
       <c r="A985" t="n">
-        <v>3600</v>
+        <v>3599</v>
       </c>
       <c r="B985" t="inlineStr">
         <is>
-          <t>29/01/2026</t>
+          <t>28/01/2026</t>
         </is>
       </c>
       <c r="C985" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D985" t="n">
         <v>4</v>
       </c>
       <c r="E985" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F985" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G985" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H985" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I985" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J985" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K985" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L985" t="n">
         <v>16</v>
       </c>
       <c r="M985" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="N985" t="n">
         <v>20</v>
@@ -54622,29 +54622,29 @@
         <v>21</v>
       </c>
       <c r="P985" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Q985" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="986">
       <c r="A986" t="n">
-        <v>3601</v>
+        <v>3600</v>
       </c>
       <c r="B986" t="inlineStr">
         <is>
-          <t>30/01/2026</t>
+          <t>29/01/2026</t>
         </is>
       </c>
       <c r="C986" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D986" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E986" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F986" t="n">
         <v>6</v>
@@ -54662,22 +54662,22 @@
         <v>11</v>
       </c>
       <c r="K986" t="n">
+        <v>12</v>
+      </c>
+      <c r="L986" t="n">
         <v>16</v>
       </c>
-      <c r="L986" t="n">
-        <v>17</v>
-      </c>
       <c r="M986" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N986" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O986" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="P986" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="Q986" t="n">
         <v>25</v>
@@ -54685,97 +54685,97 @@
     </row>
     <row r="987">
       <c r="A987" t="n">
-        <v>3602</v>
+        <v>3601</v>
       </c>
       <c r="B987" t="inlineStr">
         <is>
-          <t>31/01/2026</t>
+          <t>30/01/2026</t>
         </is>
       </c>
       <c r="C987" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D987" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E987" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F987" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G987" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H987" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I987" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J987" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="K987" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L987" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M987" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N987" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O987" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P987" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q987" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="988">
       <c r="A988" t="n">
-        <v>3603</v>
+        <v>3602</v>
       </c>
       <c r="B988" t="inlineStr">
         <is>
-          <t>02/02/2026</t>
+          <t>31/01/2026</t>
         </is>
       </c>
       <c r="C988" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D988" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E988" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F988" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G988" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H988" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="I988" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J988" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="K988" t="n">
         <v>15</v>
       </c>
       <c r="L988" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M988" t="n">
         <v>19</v>
@@ -54784,10 +54784,10 @@
         <v>20</v>
       </c>
       <c r="O988" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P988" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Q988" t="n">
         <v>24</v>
@@ -54795,54 +54795,54 @@
     </row>
     <row r="989">
       <c r="A989" t="n">
-        <v>3604</v>
+        <v>3603</v>
       </c>
       <c r="B989" t="inlineStr">
         <is>
-          <t>03/02/2026</t>
+          <t>02/02/2026</t>
         </is>
       </c>
       <c r="C989" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D989" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E989" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F989" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G989" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H989" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I989" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J989" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K989" t="n">
         <v>15</v>
       </c>
       <c r="L989" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M989" t="n">
         <v>19</v>
       </c>
       <c r="N989" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O989" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P989" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q989" t="n">
         <v>24</v>
@@ -54850,231 +54850,231 @@
     </row>
     <row r="990">
       <c r="A990" t="n">
-        <v>3605</v>
+        <v>3604</v>
       </c>
       <c r="B990" t="inlineStr">
         <is>
-          <t>04/02/2026</t>
+          <t>03/02/2026</t>
         </is>
       </c>
       <c r="C990" t="n">
         <v>1</v>
       </c>
       <c r="D990" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E990" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F990" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G990" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H990" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I990" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J990" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K990" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="L990" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="M990" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N990" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O990" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P990" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q990" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="991">
       <c r="A991" t="n">
-        <v>3606</v>
+        <v>3605</v>
       </c>
       <c r="B991" t="inlineStr">
         <is>
-          <t>05/02/2026</t>
+          <t>04/02/2026</t>
         </is>
       </c>
       <c r="C991" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D991" t="n">
         <v>3</v>
       </c>
       <c r="E991" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F991" t="n">
         <v>7</v>
       </c>
       <c r="G991" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H991" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I991" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J991" t="n">
         <v>14</v>
       </c>
       <c r="K991" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="L991" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="M991" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="N991" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O991" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="P991" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q991" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="992">
       <c r="A992" t="n">
-        <v>3607</v>
+        <v>3606</v>
       </c>
       <c r="B992" t="inlineStr">
         <is>
-          <t>06/02/2026</t>
+          <t>05/02/2026</t>
         </is>
       </c>
       <c r="C992" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D992" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E992" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F992" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G992" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H992" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I992" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J992" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K992" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L992" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="M992" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="N992" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="O992" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="P992" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="Q992" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="993">
       <c r="A993" t="n">
-        <v>3608</v>
+        <v>3607</v>
       </c>
       <c r="B993" t="inlineStr">
         <is>
-          <t>07/02/2026</t>
+          <t>06/02/2026</t>
         </is>
       </c>
       <c r="C993" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D993" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E993" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F993" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G993" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H993" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I993" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="J993" t="n">
+        <v>13</v>
+      </c>
+      <c r="K993" t="n">
+        <v>14</v>
+      </c>
+      <c r="L993" t="n">
+        <v>15</v>
+      </c>
+      <c r="M993" t="n">
         <v>16</v>
       </c>
-      <c r="K993" t="n">
-        <v>17</v>
-      </c>
-      <c r="L993" t="n">
-        <v>18</v>
-      </c>
-      <c r="M993" t="n">
-        <v>19</v>
-      </c>
       <c r="N993" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="O993" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="P993" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="Q993" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="994">
       <c r="A994" t="n">
-        <v>3609</v>
+        <v>3608</v>
       </c>
       <c r="B994" t="inlineStr">
         <is>
-          <t>09/02/2026</t>
+          <t>07/02/2026</t>
         </is>
       </c>
       <c r="C994" t="n">
@@ -55093,19 +55093,19 @@
         <v>9</v>
       </c>
       <c r="H994" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I994" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="J994" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="K994" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="L994" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M994" t="n">
         <v>19</v>
@@ -55117,7 +55117,7 @@
         <v>22</v>
       </c>
       <c r="P994" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q994" t="n">
         <v>25</v>
@@ -55125,51 +55125,51 @@
     </row>
     <row r="995">
       <c r="A995" t="n">
-        <v>3610</v>
+        <v>3609</v>
       </c>
       <c r="B995" t="inlineStr">
         <is>
-          <t>10/02/2026</t>
+          <t>09/02/2026</t>
         </is>
       </c>
       <c r="C995" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D995" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E995" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F995" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G995" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H995" t="n">
         <v>10</v>
       </c>
       <c r="I995" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J995" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K995" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="L995" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="M995" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N995" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O995" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P995" t="n">
         <v>24</v>
@@ -55180,54 +55180,54 @@
     </row>
     <row r="996">
       <c r="A996" t="n">
-        <v>3611</v>
+        <v>3610</v>
       </c>
       <c r="B996" t="inlineStr">
         <is>
-          <t>11/02/2026</t>
+          <t>10/02/2026</t>
         </is>
       </c>
       <c r="C996" t="n">
         <v>1</v>
       </c>
       <c r="D996" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E996" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F996" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G996" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H996" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I996" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J996" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="K996" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="L996" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="M996" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="N996" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="O996" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="P996" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="Q996" t="n">
         <v>25</v>
@@ -55235,54 +55235,54 @@
     </row>
     <row r="997">
       <c r="A997" t="n">
-        <v>3612</v>
+        <v>3611</v>
       </c>
       <c r="B997" t="inlineStr">
         <is>
-          <t>12/02/2026</t>
+          <t>11/02/2026</t>
         </is>
       </c>
       <c r="C997" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D997" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E997" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F997" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G997" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="H997" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="I997" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J997" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="K997" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="L997" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="M997" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="N997" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="O997" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="P997" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="Q997" t="n">
         <v>25</v>
@@ -55290,45 +55290,45 @@
     </row>
     <row r="998">
       <c r="A998" t="n">
-        <v>3613</v>
+        <v>3612</v>
       </c>
       <c r="B998" t="inlineStr">
         <is>
-          <t>13/02/2026</t>
+          <t>12/02/2026</t>
         </is>
       </c>
       <c r="C998" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D998" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E998" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F998" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G998" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H998" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="I998" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="J998" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="K998" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="L998" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M998" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N998" t="n">
         <v>20</v>
@@ -55340,29 +55340,29 @@
         <v>22</v>
       </c>
       <c r="Q998" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="999">
       <c r="A999" t="n">
-        <v>3614</v>
+        <v>3613</v>
       </c>
       <c r="B999" t="inlineStr">
         <is>
-          <t>14/02/2026</t>
+          <t>13/02/2026</t>
         </is>
       </c>
       <c r="C999" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D999" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E999" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F999" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G999" t="n">
         <v>9</v>
@@ -55377,79 +55377,134 @@
         <v>12</v>
       </c>
       <c r="K999" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L999" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M999" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="N999" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="O999" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P999" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q999" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="1000">
       <c r="A1000" t="n">
+        <v>3614</v>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>14/02/2026</t>
+        </is>
+      </c>
+      <c r="C1000" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1000" t="n">
+        <v>4</v>
+      </c>
+      <c r="E1000" t="n">
+        <v>5</v>
+      </c>
+      <c r="F1000" t="n">
+        <v>6</v>
+      </c>
+      <c r="G1000" t="n">
+        <v>9</v>
+      </c>
+      <c r="H1000" t="n">
+        <v>10</v>
+      </c>
+      <c r="I1000" t="n">
+        <v>11</v>
+      </c>
+      <c r="J1000" t="n">
+        <v>12</v>
+      </c>
+      <c r="K1000" t="n">
+        <v>14</v>
+      </c>
+      <c r="L1000" t="n">
+        <v>15</v>
+      </c>
+      <c r="M1000" t="n">
+        <v>16</v>
+      </c>
+      <c r="N1000" t="n">
+        <v>17</v>
+      </c>
+      <c r="O1000" t="n">
+        <v>20</v>
+      </c>
+      <c r="P1000" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q1000" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="n">
         <v>3615</v>
       </c>
-      <c r="B1000" t="inlineStr">
+      <c r="B1001" t="inlineStr">
         <is>
           <t>18/02/2026</t>
         </is>
       </c>
-      <c r="C1000" t="n">
-        <v>2</v>
-      </c>
-      <c r="D1000" t="n">
-        <v>3</v>
-      </c>
-      <c r="E1000" t="n">
-        <v>6</v>
-      </c>
-      <c r="F1000" t="n">
-        <v>7</v>
-      </c>
-      <c r="G1000" t="n">
-        <v>8</v>
-      </c>
-      <c r="H1000" t="n">
-        <v>9</v>
-      </c>
-      <c r="I1000" t="n">
-        <v>10</v>
-      </c>
-      <c r="J1000" t="n">
-        <v>11</v>
-      </c>
-      <c r="K1000" t="n">
-        <v>14</v>
-      </c>
-      <c r="L1000" t="n">
-        <v>15</v>
-      </c>
-      <c r="M1000" t="n">
-        <v>17</v>
-      </c>
-      <c r="N1000" t="n">
-        <v>18</v>
-      </c>
-      <c r="O1000" t="n">
-        <v>21</v>
-      </c>
-      <c r="P1000" t="n">
-        <v>23</v>
-      </c>
-      <c r="Q1000" t="n">
+      <c r="C1001" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1001" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1001" t="n">
+        <v>6</v>
+      </c>
+      <c r="F1001" t="n">
+        <v>7</v>
+      </c>
+      <c r="G1001" t="n">
+        <v>8</v>
+      </c>
+      <c r="H1001" t="n">
+        <v>9</v>
+      </c>
+      <c r="I1001" t="n">
+        <v>10</v>
+      </c>
+      <c r="J1001" t="n">
+        <v>11</v>
+      </c>
+      <c r="K1001" t="n">
+        <v>14</v>
+      </c>
+      <c r="L1001" t="n">
+        <v>15</v>
+      </c>
+      <c r="M1001" t="n">
+        <v>17</v>
+      </c>
+      <c r="N1001" t="n">
+        <v>18</v>
+      </c>
+      <c r="O1001" t="n">
+        <v>21</v>
+      </c>
+      <c r="P1001" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q1001" t="n">
         <v>25</v>
       </c>
     </row>

</xml_diff>